<commit_message>
Update 1st Sprint Complete
</commit_message>
<xml_diff>
--- a/ConfigFile/Config.xlsx
+++ b/ConfigFile/Config.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>C:\Users\Patcharin.K\Documents\UiPath\PPMS_Automation\ConfigFile\</t>
+  </si>
+  <si>
+    <t>blankTemplatePath</t>
+  </si>
+  <si>
+    <t>ไฟล์ Template ที่มี Header ของ Log</t>
+  </si>
+  <si>
+    <t>ไฟล์ Template เปล่าๆ ไว้ใส่ข้อมูลที่ Log แล้ว</t>
+  </si>
+  <si>
+    <t>logPath</t>
+  </si>
+  <si>
+    <t>ไฟล์เก็บ Log</t>
+  </si>
+  <si>
+    <t>D:\Mean\UIpath Workspace\Output\log\</t>
   </si>
 </sst>
 </file>
@@ -179,12 +197,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -602,7 +621,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,17 +715,31 @@
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -725,6 +758,7 @@
     <hyperlink ref="B7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>